<commit_message>
change calc_ypll to aggregate_date.R
</commit_message>
<xml_diff>
--- a/inst/impute/results/covid19deaths_impute_age_group2.xlsx
+++ b/inst/impute/results/covid19deaths_impute_age_group2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">age_group</t>
   </si>
@@ -20,9 +20,6 @@
     <t xml:space="preserve">sum_covid19_deaths</t>
   </si>
   <si>
-    <t xml:space="preserve">sum_ypll</t>
-  </si>
-  <si>
     <t xml:space="preserve">type</t>
   </si>
   <si>
@@ -30,12 +27,6 @@
   </si>
   <si>
     <t xml:space="preserve">ub_d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lb_ypll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ub_ypll</t>
   </si>
   <si>
     <t xml:space="preserve">covid_19_deaths</t>
@@ -425,630 +416,460 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>347</v>
       </c>
-      <c r="C2" t="n">
-        <v>1187.93840728997</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2"/>
       <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2" t="n">
+      <c r="F2" t="n">
         <v>1476</v>
       </c>
-      <c r="J2" t="n">
+      <c r="G2" t="n">
         <v>-76.49</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" t="n">
         <v>1701</v>
       </c>
-      <c r="C3" t="n">
-        <v>9882.09242957526</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3"/>
       <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3" t="n">
+      <c r="F3" t="n">
         <v>4272</v>
       </c>
-      <c r="J3" t="n">
+      <c r="G3" t="n">
         <v>-60.18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" t="n">
         <v>5992</v>
       </c>
-      <c r="C4" t="n">
-        <v>42112.842276823</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4"/>
       <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4" t="n">
+      <c r="F4" t="n">
         <v>11291</v>
       </c>
-      <c r="J4" t="n">
+      <c r="G4" t="n">
         <v>-46.93</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" t="n">
         <v>42538</v>
       </c>
-      <c r="C5" t="n">
-        <v>335858.550338804</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5"/>
       <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5" t="n">
+      <c r="F5" t="n">
         <v>56630</v>
       </c>
-      <c r="J5" t="n">
+      <c r="G5" t="n">
         <v>-24.88</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" t="n">
         <v>65905</v>
       </c>
-      <c r="C6" t="n">
-        <v>469911.860960396</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6"/>
       <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6" t="n">
+      <c r="F6" t="n">
         <v>82059</v>
       </c>
-      <c r="J6" t="n">
+      <c r="G6" t="n">
         <v>-19.69</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7" t="n">
         <v>89367</v>
       </c>
-      <c r="C7" t="n">
-        <v>703336.494094044</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7"/>
       <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7" t="n">
+      <c r="F7" t="n">
         <v>105964</v>
       </c>
-      <c r="J7" t="n">
+      <c r="G7" t="n">
         <v>-15.66</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B8" t="n">
         <v>107056</v>
       </c>
-      <c r="C8" t="n">
-        <v>436932.395691759</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8"/>
       <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8" t="n">
+      <c r="F8" t="n">
         <v>122488</v>
       </c>
-      <c r="J8" t="n">
+      <c r="G8" t="n">
         <v>-12.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" t="n">
         <v>1456.769</v>
       </c>
-      <c r="C9" t="n">
-        <v>90391.6437519407</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1412</v>
       </c>
       <c r="E9" t="n">
-        <v>1412</v>
+        <v>1505.025</v>
       </c>
       <c r="F9" t="n">
-        <v>1505.025</v>
+        <v>1476</v>
       </c>
       <c r="G9" t="n">
-        <v>89711.0551257234</v>
-      </c>
-      <c r="H9" t="n">
-        <v>91174.7378791243</v>
-      </c>
-      <c r="I9" t="n">
-        <v>1476</v>
-      </c>
-      <c r="J9" t="n">
         <v>-1.3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" t="n">
         <v>4567.355</v>
       </c>
-      <c r="C10" t="n">
-        <v>292454.500463424</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="n">
+        <v>4472.975</v>
       </c>
       <c r="E10" t="n">
-        <v>4472.975</v>
+        <v>4662</v>
       </c>
       <c r="F10" t="n">
-        <v>4662</v>
+        <v>4272</v>
       </c>
       <c r="G10" t="n">
-        <v>288396.594663533</v>
-      </c>
-      <c r="H10" t="n">
-        <v>297155.568407077</v>
-      </c>
-      <c r="I10" t="n">
-        <v>4272</v>
-      </c>
-      <c r="J10" t="n">
         <v>6.91</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B11" t="n">
         <v>12269.823</v>
       </c>
-      <c r="C11" t="n">
-        <v>724642.960716415</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="n">
+        <v>12107.9</v>
       </c>
       <c r="E11" t="n">
-        <v>12107.9</v>
+        <v>12451.15</v>
       </c>
       <c r="F11" t="n">
-        <v>12451.15</v>
+        <v>11291</v>
       </c>
       <c r="G11" t="n">
-        <v>706441.24660383</v>
-      </c>
-      <c r="H11" t="n">
-        <v>743780.133789601</v>
-      </c>
-      <c r="I11" t="n">
-        <v>11291</v>
-      </c>
-      <c r="J11" t="n">
         <v>8.67</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B12" t="n">
         <v>59055.111</v>
       </c>
-      <c r="C12" t="n">
-        <v>2052487.12314353</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="n">
+        <v>58729</v>
       </c>
       <c r="E12" t="n">
-        <v>58729</v>
+        <v>59367.05</v>
       </c>
       <c r="F12" t="n">
-        <v>59367.05</v>
+        <v>56630</v>
       </c>
       <c r="G12" t="n">
-        <v>2006297.10258734</v>
-      </c>
-      <c r="H12" t="n">
-        <v>2100264.54712826</v>
-      </c>
-      <c r="I12" t="n">
-        <v>56630</v>
-      </c>
-      <c r="J12" t="n">
         <v>4.28</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B13" t="n">
         <v>85092.008</v>
       </c>
-      <c r="C13" t="n">
-        <v>1831508.36814558</v>
-      </c>
-      <c r="D13" t="s">
-        <v>18</v>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="n">
+        <v>84745</v>
       </c>
       <c r="E13" t="n">
-        <v>84745</v>
+        <v>85476.025</v>
       </c>
       <c r="F13" t="n">
-        <v>85476.025</v>
+        <v>82059</v>
       </c>
       <c r="G13" t="n">
-        <v>1796327.34563762</v>
-      </c>
-      <c r="H13" t="n">
-        <v>1869749.2099043</v>
-      </c>
-      <c r="I13" t="n">
-        <v>82059</v>
-      </c>
-      <c r="J13" t="n">
         <v>3.7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B14" t="n">
         <v>109408.771</v>
       </c>
-      <c r="C14" t="n">
-        <v>2031565.74096556</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="n">
+        <v>109071.8</v>
       </c>
       <c r="E14" t="n">
-        <v>109071.8</v>
+        <v>109756.1</v>
       </c>
       <c r="F14" t="n">
-        <v>109756.1</v>
+        <v>105964</v>
       </c>
       <c r="G14" t="n">
-        <v>1997498.52027891</v>
-      </c>
-      <c r="H14" t="n">
-        <v>2066800.22094964</v>
-      </c>
-      <c r="I14" t="n">
-        <v>105964</v>
-      </c>
-      <c r="J14" t="n">
         <v>3.25</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B15" t="n">
         <v>126341.76</v>
       </c>
-      <c r="C15" t="n">
-        <v>1122908.0087308</v>
-      </c>
-      <c r="D15" t="s">
-        <v>18</v>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="n">
+        <v>126014.925</v>
       </c>
       <c r="E15" t="n">
-        <v>126014.925</v>
+        <v>126667.1</v>
       </c>
       <c r="F15" t="n">
-        <v>126667.1</v>
+        <v>122488</v>
       </c>
       <c r="G15" t="n">
-        <v>1104329.88578378</v>
-      </c>
-      <c r="H15" t="n">
-        <v>1142006.28647796</v>
-      </c>
-      <c r="I15" t="n">
-        <v>122488</v>
-      </c>
-      <c r="J15" t="n">
         <v>3.15</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B16" t="n">
-        <v>3948.082</v>
-      </c>
-      <c r="C16" t="n">
-        <v>428559.687684434</v>
-      </c>
-      <c r="D16" t="s">
-        <v>19</v>
+        <v>3955.479</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3831.925</v>
       </c>
       <c r="E16" t="n">
-        <v>3818.975</v>
+        <v>4091.025</v>
       </c>
       <c r="F16" t="n">
-        <v>4073.075</v>
+        <v>1476</v>
       </c>
       <c r="G16" t="n">
-        <v>394789.815926462</v>
-      </c>
-      <c r="H16" t="n">
-        <v>460844.171140245</v>
-      </c>
-      <c r="I16" t="n">
-        <v>1476</v>
-      </c>
-      <c r="J16" t="n">
-        <v>167.49</v>
+        <v>167.99</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B17" t="n">
-        <v>8755.23</v>
-      </c>
-      <c r="C17" t="n">
-        <v>1256824.92419938</v>
-      </c>
-      <c r="D17" t="s">
-        <v>19</v>
+        <v>8758.064</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="n">
+        <v>8574.975</v>
       </c>
       <c r="E17" t="n">
-        <v>8560.975</v>
+        <v>8932.05</v>
       </c>
       <c r="F17" t="n">
-        <v>8934</v>
+        <v>4272</v>
       </c>
       <c r="G17" t="n">
-        <v>1178401.17684834</v>
-      </c>
-      <c r="H17" t="n">
-        <v>1337025.96018734</v>
-      </c>
-      <c r="I17" t="n">
-        <v>4272</v>
-      </c>
-      <c r="J17" t="n">
-        <v>104.94</v>
+        <v>105.01</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B18" t="n">
-        <v>18299.433</v>
-      </c>
-      <c r="C18" t="n">
-        <v>2404600.64026652</v>
-      </c>
-      <c r="D18" t="s">
-        <v>19</v>
+        <v>18294.811</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="n">
+        <v>18033.95</v>
       </c>
       <c r="E18" t="n">
-        <v>18046.95</v>
+        <v>18545.05</v>
       </c>
       <c r="F18" t="n">
-        <v>18553.025</v>
+        <v>11291</v>
       </c>
       <c r="G18" t="n">
-        <v>2309391.68229295</v>
-      </c>
-      <c r="H18" t="n">
-        <v>2504005.79365676</v>
-      </c>
-      <c r="I18" t="n">
-        <v>11291</v>
-      </c>
-      <c r="J18" t="n">
-        <v>62.07</v>
+        <v>62.03</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B19" t="n">
-        <v>65762.378</v>
-      </c>
-      <c r="C19" t="n">
-        <v>3729316.2190847</v>
-      </c>
-      <c r="D19" t="s">
-        <v>19</v>
+        <v>65776.038</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" t="n">
+        <v>65442.95</v>
       </c>
       <c r="E19" t="n">
-        <v>65417</v>
+        <v>66091.125</v>
       </c>
       <c r="F19" t="n">
-        <v>66099.1</v>
+        <v>56630</v>
       </c>
       <c r="G19" t="n">
-        <v>3628652.34651993</v>
-      </c>
-      <c r="H19" t="n">
-        <v>3824050.24152115</v>
-      </c>
-      <c r="I19" t="n">
-        <v>56630</v>
-      </c>
-      <c r="J19" t="n">
-        <v>16.13</v>
+        <v>16.15</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B20" t="n">
-        <v>90356.104</v>
-      </c>
-      <c r="C20" t="n">
-        <v>2753561.52080426</v>
-      </c>
-      <c r="D20" t="s">
-        <v>19</v>
+        <v>90348.185</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="n">
+        <v>90008.9</v>
       </c>
       <c r="E20" t="n">
-        <v>90006</v>
+        <v>90713.125</v>
       </c>
       <c r="F20" t="n">
-        <v>90707</v>
+        <v>82059</v>
       </c>
       <c r="G20" t="n">
-        <v>2688759.47843273</v>
-      </c>
-      <c r="H20" t="n">
-        <v>2819801.09118252</v>
-      </c>
-      <c r="I20" t="n">
-        <v>82059</v>
-      </c>
-      <c r="J20" t="n">
-        <v>10.11</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="n">
+        <v>113345.491</v>
+      </c>
+      <c r="C21" t="s">
         <v>16</v>
       </c>
-      <c r="B21" t="n">
-        <v>113351.098</v>
-      </c>
-      <c r="C21" t="n">
-        <v>2632161.27080289</v>
-      </c>
-      <c r="D21" t="s">
-        <v>19</v>
+      <c r="D21" t="n">
+        <v>113006.975</v>
       </c>
       <c r="E21" t="n">
-        <v>112999.925</v>
+        <v>113698.1</v>
       </c>
       <c r="F21" t="n">
-        <v>113696.075</v>
+        <v>105964</v>
       </c>
       <c r="G21" t="n">
-        <v>2581301.26988828</v>
-      </c>
-      <c r="H21" t="n">
-        <v>2679987.94977389</v>
-      </c>
-      <c r="I21" t="n">
-        <v>105964</v>
-      </c>
-      <c r="J21" t="n">
         <v>6.97</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B22" t="n">
-        <v>129205.962</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1388431.63383603</v>
-      </c>
-      <c r="D22" t="s">
-        <v>19</v>
+        <v>129184.021</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" t="n">
+        <v>128867</v>
       </c>
       <c r="E22" t="n">
-        <v>128838.925</v>
+        <v>129532.075</v>
       </c>
       <c r="F22" t="n">
-        <v>129528.175</v>
+        <v>122488</v>
       </c>
       <c r="G22" t="n">
-        <v>1358851.41287209</v>
-      </c>
-      <c r="H22" t="n">
-        <v>1417364.03970183</v>
-      </c>
-      <c r="I22" t="n">
-        <v>122488</v>
-      </c>
-      <c r="J22" t="n">
-        <v>5.48</v>
+        <v>5.47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clear and clean results
</commit_message>
<xml_diff>
--- a/inst/impute/results/covid19deaths_impute_age_group2.xlsx
+++ b/inst/impute/results/covid19deaths_impute_age_group2.xlsx
@@ -716,22 +716,22 @@
         <v>7</v>
       </c>
       <c r="B16" t="n">
-        <v>3955.479</v>
+        <v>3950.205</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="n">
-        <v>3831.925</v>
+        <v>3810.975</v>
       </c>
       <c r="E16" t="n">
-        <v>4091.025</v>
+        <v>4085</v>
       </c>
       <c r="F16" t="n">
         <v>1476</v>
       </c>
       <c r="G16" t="n">
-        <v>167.99</v>
+        <v>167.63</v>
       </c>
     </row>
     <row r="17">
@@ -739,16 +739,16 @@
         <v>9</v>
       </c>
       <c r="B17" t="n">
-        <v>8758.064</v>
+        <v>8758.209</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>8574.975</v>
+        <v>8566.975</v>
       </c>
       <c r="E17" t="n">
-        <v>8932.05</v>
+        <v>8950.025</v>
       </c>
       <c r="F17" t="n">
         <v>4272</v>
@@ -762,22 +762,22 @@
         <v>10</v>
       </c>
       <c r="B18" t="n">
-        <v>18294.811</v>
+        <v>18304.913</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
       </c>
       <c r="D18" t="n">
-        <v>18033.95</v>
+        <v>18068.975</v>
       </c>
       <c r="E18" t="n">
-        <v>18545.05</v>
+        <v>18562.075</v>
       </c>
       <c r="F18" t="n">
         <v>11291</v>
       </c>
       <c r="G18" t="n">
-        <v>62.03</v>
+        <v>62.12</v>
       </c>
     </row>
     <row r="19">
@@ -785,16 +785,16 @@
         <v>11</v>
       </c>
       <c r="B19" t="n">
-        <v>65776.038</v>
+        <v>65777.407</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
       </c>
       <c r="D19" t="n">
-        <v>65442.95</v>
+        <v>65426.975</v>
       </c>
       <c r="E19" t="n">
-        <v>66091.125</v>
+        <v>66119.075</v>
       </c>
       <c r="F19" t="n">
         <v>56630</v>
@@ -808,22 +808,22 @@
         <v>12</v>
       </c>
       <c r="B20" t="n">
-        <v>90348.185</v>
+        <v>90358.363</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
       </c>
       <c r="D20" t="n">
-        <v>90008.9</v>
+        <v>90011.9</v>
       </c>
       <c r="E20" t="n">
-        <v>90713.125</v>
+        <v>90696.175</v>
       </c>
       <c r="F20" t="n">
         <v>82059</v>
       </c>
       <c r="G20" t="n">
-        <v>10.1</v>
+        <v>10.11</v>
       </c>
     </row>
     <row r="21">
@@ -831,22 +831,22 @@
         <v>13</v>
       </c>
       <c r="B21" t="n">
-        <v>113345.491</v>
+        <v>113356.84</v>
       </c>
       <c r="C21" t="s">
         <v>16</v>
       </c>
       <c r="D21" t="n">
-        <v>113006.975</v>
+        <v>112999.9</v>
       </c>
       <c r="E21" t="n">
-        <v>113698.1</v>
+        <v>113699</v>
       </c>
       <c r="F21" t="n">
         <v>105964</v>
       </c>
       <c r="G21" t="n">
-        <v>6.97</v>
+        <v>6.98</v>
       </c>
     </row>
     <row r="22">
@@ -854,22 +854,22 @@
         <v>14</v>
       </c>
       <c r="B22" t="n">
-        <v>129184.021</v>
+        <v>129195.39</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
       </c>
       <c r="D22" t="n">
-        <v>128867</v>
+        <v>128871.975</v>
       </c>
       <c r="E22" t="n">
-        <v>129532.075</v>
+        <v>129540</v>
       </c>
       <c r="F22" t="n">
         <v>122488</v>
       </c>
       <c r="G22" t="n">
-        <v>5.47</v>
+        <v>5.48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>